<commit_message>
Added closed bookings and some other stuff....its too late can't think
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/file/question_template.xlsx
+++ b/src/main/webapp/resources/file/question_template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t xml:space="preserve">Question Type</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t xml:space="preserve">Correct Answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Length(seconds)</t>
   </si>
   <si>
     <t xml:space="preserve">Empty</t>
@@ -71,6 +74,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -92,6 +96,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -263,21 +268,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -302,10 +308,13 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -313,10 +322,11 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -324,10 +334,11 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -335,10 +346,11 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -346,10 +358,11 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -357,10 +370,11 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -368,10 +382,11 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -379,10 +394,11 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -390,10 +406,11 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -401,6 +418,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -434,22 +452,22 @@
       <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>2</v>
@@ -457,7 +475,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>3</v>
@@ -476,7 +494,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>